<commit_message>
add new tcs account settings, registration, login
</commit_message>
<xml_diff>
--- a/Data/Credential/Login.xlsx
+++ b/Data/Credential/Login.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation Project\gocad-automation-katalon\Data\Credential\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F01583AC-EF05-4CD0-A64F-ED2764ADC55C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{751F0DE0-6AAF-450D-88E5-A35EFE057EAB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="495" windowWidth="28800" windowHeight="16425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="AC-FA007297" sheetId="4" r:id="rId1"/>
+    <sheet name="UI" sheetId="5" r:id="rId1"/>
+    <sheet name="API" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="18">
   <si>
     <t>systemRole</t>
   </si>
@@ -50,6 +51,30 @@
   </si>
   <si>
     <t>can login system successfully</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>inputExpected</t>
+  </si>
+  <si>
+    <t>abcd</t>
+  </si>
+  <si>
+    <t>sdfgds@gmail.com</t>
+  </si>
+  <si>
+    <t>errorSystem</t>
+  </si>
+  <si>
+    <t>errorUI</t>
+  </si>
+  <si>
+    <t>truongbaothuy93@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -110,7 +135,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -118,6 +143,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -394,10 +422,91 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F68D1E8-125A-4BC9-BEF7-9617A167D0F0}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="2" width="31.140625" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="3"/>
+      <c r="B4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="3"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1" xr:uid="{34182B3B-A3AB-447D-81F0-486986903894}"/>
+    <hyperlink ref="A5" r:id="rId2" xr:uid="{A0059E35-AFF8-49B4-89CF-362EB4B033ED}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>

</xml_diff>